<commit_message>
- changed bitfield values to sbyte values for easier encoding and decoding - added conversion class to convert current datapool to raw byte array - finished adding first basic set of car values - added test class to check for id problems, like duplicates
</commit_message>
<xml_diff>
--- a/docs/TelemetryValues.xlsx
+++ b/docs/TelemetryValues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Code\Telemetry Reader\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD48BFB2-F081-46A5-9654-E7CFD0C2D907}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741BF660-DF4C-40F4-9C6B-32F0247E05D0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17565" xr2:uid="{A755A8CE-3DDE-4B04-B560-9846973B1798}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="178">
   <si>
     <t>Title</t>
   </si>
@@ -495,24 +495,6 @@
     <t>On / Off</t>
   </si>
   <si>
-    <t>8-bit Bitfield - 606/1</t>
-  </si>
-  <si>
-    <t>8-bit Bitfield - 615/1</t>
-  </si>
-  <si>
-    <t>8-bit Bitfield - 606/2</t>
-  </si>
-  <si>
-    <t>8-bit Bitfield - 606/3</t>
-  </si>
-  <si>
-    <t>8-bit Bitfield - 606/4</t>
-  </si>
-  <si>
-    <t>8-bit Bitfield - 612/1</t>
-  </si>
-  <si>
     <t>Engine Active</t>
   </si>
   <si>
@@ -534,45 +516,12 @@
     <t>Water Temperature Warning</t>
   </si>
   <si>
-    <t>8-bit Bitfield - 615/2</t>
-  </si>
-  <si>
-    <t>8-bit Bitfield - 615/3</t>
-  </si>
-  <si>
-    <t>8-bit Bitfield - 615/4</t>
-  </si>
-  <si>
-    <t>8-bit Bitfield - 615/5</t>
-  </si>
-  <si>
-    <t>8-bit Bitfield - 615/6</t>
-  </si>
-  <si>
-    <t>8-bit Bitfield - 615/0</t>
-  </si>
-  <si>
-    <t>8-bit Bitfield - 606/0</t>
-  </si>
-  <si>
-    <t>8-bit Bitfield - 612/0</t>
-  </si>
-  <si>
     <t>Fuel Pressure Warning</t>
   </si>
   <si>
     <t>Information</t>
   </si>
   <si>
-    <t>8-bit Bitfield - 615/7</t>
-  </si>
-  <si>
-    <t>8-bit Bitfield - 612/2</t>
-  </si>
-  <si>
-    <t>8-bit Bitfield - 612/3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pit Limiter </t>
   </si>
   <si>
@@ -594,24 +543,15 @@
     <t>Drag Reduction System</t>
   </si>
   <si>
-    <t>8-bit Bitfield - 612/4</t>
-  </si>
-  <si>
     <t>Rev limiter</t>
   </si>
   <si>
-    <t>8-bit Bitfield - 612/5</t>
-  </si>
-  <si>
     <t>Stability Control Level</t>
   </si>
   <si>
     <t>Stability Control</t>
   </si>
   <si>
-    <t>8-bit Bitfield - 612/6</t>
-  </si>
-  <si>
     <t>Traction Control Level 1</t>
   </si>
   <si>
@@ -619,9 +559,6 @@
   </si>
   <si>
     <t>Traction Control</t>
-  </si>
-  <si>
-    <t>8-bit Bitfield - 612/7</t>
   </si>
   <si>
     <t>Electronics</t>
@@ -694,7 +631,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -714,6 +651,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -2076,8 +2017,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="0" y="68648"/>
-          <a:ext cx="6613993" cy="3695674"/>
+          <a:off x="0" y="57162"/>
+          <a:ext cx="6596063" cy="3695674"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -2118,7 +2059,7 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="513319" tIns="708152" rIns="513319" bIns="113792" numCol="1" spcCol="1270" anchor="t" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="511928" tIns="708152" rIns="511928" bIns="113792" numCol="1" spcCol="1270" anchor="t" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -2268,8 +2209,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="180408" y="249056"/>
-        <a:ext cx="6253177" cy="3334858"/>
+        <a:off x="180408" y="237570"/>
+        <a:ext cx="6235247" cy="3334858"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{4A60E55B-EC82-44B0-A838-A5F0B91A2AD9}">
@@ -2279,8 +2220,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="716216" y="0"/>
-          <a:ext cx="4629795" cy="765347"/>
+          <a:off x="714274" y="0"/>
+          <a:ext cx="4617244" cy="765347"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -2352,7 +2293,7 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="174995" tIns="0" rIns="174995" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="174521" tIns="0" rIns="174521" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -2376,8 +2317,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="753577" y="37361"/>
-        <a:ext cx="4555073" cy="690625"/>
+        <a:off x="751635" y="37361"/>
+        <a:ext cx="4542522" cy="690625"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -3946,8 +3887,8 @@
   </sheetPr>
   <dimension ref="A1:I1538"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -6119,23 +6060,23 @@
         <v>104</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A96" s="7" t="s">
+    <row r="96" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="10">
         <v>606</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D96" t="s">
-        <v>172</v>
-      </c>
-      <c r="E96" t="s">
+        <v>26</v>
+      </c>
+      <c r="E96" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="G96" t="s">
+      <c r="G96" s="8" t="s">
         <v>147</v>
       </c>
     </row>
@@ -6150,7 +6091,7 @@
         <v>146</v>
       </c>
       <c r="D97" t="s">
-        <v>153</v>
+        <v>26</v>
       </c>
       <c r="E97" t="s">
         <v>148</v>
@@ -6170,7 +6111,7 @@
         <v>146</v>
       </c>
       <c r="D98" t="s">
-        <v>155</v>
+        <v>26</v>
       </c>
       <c r="E98" t="s">
         <v>148</v>
@@ -6190,7 +6131,7 @@
         <v>146</v>
       </c>
       <c r="D99" t="s">
-        <v>156</v>
+        <v>26</v>
       </c>
       <c r="E99" t="s">
         <v>148</v>
@@ -6210,7 +6151,7 @@
         <v>146</v>
       </c>
       <c r="D100" t="s">
-        <v>157</v>
+        <v>26</v>
       </c>
       <c r="E100" t="s">
         <v>148</v>
@@ -6236,18 +6177,18 @@
         <v>149</v>
       </c>
       <c r="F101" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="G101" t="s">
         <v>23</v>
       </c>
       <c r="H101" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" s="7" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="B102" s="1">
         <v>612</v>
@@ -6256,19 +6197,19 @@
         <v>146</v>
       </c>
       <c r="D102" t="s">
-        <v>173</v>
+        <v>26</v>
       </c>
       <c r="E102" t="s">
         <v>149</v>
       </c>
       <c r="F102" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="G102" t="s">
         <v>152</v>
       </c>
       <c r="H102" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
@@ -6288,18 +6229,18 @@
         <v>149</v>
       </c>
       <c r="F103" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="G103" t="s">
         <v>23</v>
       </c>
       <c r="H103" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" s="7" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="B104" s="1">
         <v>614</v>
@@ -6308,24 +6249,24 @@
         <v>146</v>
       </c>
       <c r="D104" t="s">
-        <v>158</v>
+        <v>26</v>
       </c>
       <c r="E104" t="s">
         <v>149</v>
       </c>
       <c r="F104" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="G104" t="s">
         <v>152</v>
       </c>
       <c r="H104" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" s="7" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B105" s="1">
         <v>615</v>
@@ -6334,10 +6275,10 @@
         <v>146</v>
       </c>
       <c r="D105" t="s">
-        <v>171</v>
+        <v>26</v>
       </c>
       <c r="E105" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="G105" t="s">
         <v>147</v>
@@ -6346,7 +6287,7 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" s="7" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B106" s="1">
         <v>616</v>
@@ -6355,10 +6296,10 @@
         <v>146</v>
       </c>
       <c r="D106" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="E106" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="G106" t="s">
         <v>147</v>
@@ -6367,7 +6308,7 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" s="7" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B107" s="1">
         <v>617</v>
@@ -6376,10 +6317,10 @@
         <v>146</v>
       </c>
       <c r="D107" t="s">
-        <v>166</v>
+        <v>26</v>
       </c>
       <c r="E107" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="G107" t="s">
         <v>147</v>
@@ -6388,7 +6329,7 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" s="7" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B108" s="1">
         <v>618</v>
@@ -6397,10 +6338,10 @@
         <v>146</v>
       </c>
       <c r="D108" t="s">
-        <v>167</v>
+        <v>26</v>
       </c>
       <c r="E108" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="G108" t="s">
         <v>147</v>
@@ -6409,7 +6350,7 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" s="7" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B109" s="1">
         <v>619</v>
@@ -6418,10 +6359,10 @@
         <v>146</v>
       </c>
       <c r="D109" t="s">
-        <v>168</v>
+        <v>26</v>
       </c>
       <c r="E109" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="G109" t="s">
         <v>147</v>
@@ -6430,7 +6371,7 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" s="7" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B110" s="1">
         <v>620</v>
@@ -6439,10 +6380,10 @@
         <v>146</v>
       </c>
       <c r="D110" t="s">
-        <v>169</v>
+        <v>26</v>
       </c>
       <c r="E110" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="G110" t="s">
         <v>147</v>
@@ -6451,7 +6392,7 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" s="7" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B111" s="1">
         <v>621</v>
@@ -6460,10 +6401,10 @@
         <v>146</v>
       </c>
       <c r="D111" t="s">
-        <v>170</v>
+        <v>26</v>
       </c>
       <c r="E111" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="G111" t="s">
         <v>147</v>
@@ -6472,7 +6413,7 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" s="7" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="B112" s="1">
         <v>622</v>
@@ -6481,42 +6422,42 @@
         <v>146</v>
       </c>
       <c r="D112" t="s">
-        <v>176</v>
+        <v>26</v>
       </c>
       <c r="E112" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="G112" t="s">
         <v>147</v>
       </c>
       <c r="I112" s="5"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A113" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="B113" s="1">
+    <row r="113" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A113" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B113" s="10">
         <v>623</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D113" t="s">
-        <v>177</v>
-      </c>
-      <c r="E113" t="s">
+        <v>26</v>
+      </c>
+      <c r="E113" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="F113" t="s">
-        <v>196</v>
-      </c>
-      <c r="G113" t="s">
+      <c r="F113" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="G113" s="8" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114" s="7" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="B114" s="1">
         <v>624</v>
@@ -6525,13 +6466,13 @@
         <v>146</v>
       </c>
       <c r="D114" t="s">
-        <v>178</v>
+        <v>26</v>
       </c>
       <c r="E114" t="s">
         <v>149</v>
       </c>
       <c r="F114" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="G114" t="s">
         <v>152</v>
@@ -6539,7 +6480,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A115" s="7" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="B115" s="1">
         <v>625</v>
@@ -6548,13 +6489,13 @@
         <v>146</v>
       </c>
       <c r="D115" t="s">
-        <v>186</v>
+        <v>26</v>
       </c>
       <c r="E115" t="s">
         <v>149</v>
       </c>
       <c r="F115" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="G115" t="s">
         <v>152</v>
@@ -6562,7 +6503,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A116" s="7" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="B116" s="1">
         <v>626</v>
@@ -6571,13 +6512,13 @@
         <v>146</v>
       </c>
       <c r="D116" t="s">
-        <v>188</v>
+        <v>26</v>
       </c>
       <c r="E116" t="s">
         <v>149</v>
       </c>
       <c r="F116" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="G116" t="s">
         <v>152</v>
@@ -6585,7 +6526,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117" s="7" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="B117" s="1">
         <v>627</v>
@@ -6600,7 +6541,7 @@
         <v>149</v>
       </c>
       <c r="F117" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="G117" t="s">
         <v>23</v>
@@ -6608,7 +6549,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A118" s="7" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="B118" s="1">
         <v>628</v>
@@ -6617,13 +6558,13 @@
         <v>146</v>
       </c>
       <c r="D118" t="s">
-        <v>191</v>
+        <v>26</v>
       </c>
       <c r="E118" t="s">
         <v>149</v>
       </c>
       <c r="F118" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="G118" t="s">
         <v>152</v>
@@ -6631,7 +6572,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A119" s="7" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="B119" s="1">
         <v>629</v>
@@ -6646,7 +6587,7 @@
         <v>149</v>
       </c>
       <c r="F119" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="G119" t="s">
         <v>23</v>
@@ -6654,7 +6595,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A120" s="7" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="B120" s="1">
         <v>630</v>
@@ -6669,7 +6610,7 @@
         <v>149</v>
       </c>
       <c r="F120" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="G120" t="s">
         <v>23</v>
@@ -6677,7 +6618,7 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A121" s="7" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="B121" s="1">
         <v>631</v>
@@ -6686,13 +6627,13 @@
         <v>146</v>
       </c>
       <c r="D121" t="s">
-        <v>195</v>
+        <v>26</v>
       </c>
       <c r="E121" t="s">
         <v>149</v>
       </c>
       <c r="F121" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="G121" t="s">
         <v>152</v>
@@ -6700,7 +6641,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A122" s="7" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="B122" s="1">
         <v>632</v>
@@ -6715,7 +6656,7 @@
         <v>149</v>
       </c>
       <c r="F122" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="G122" t="s">
         <v>12</v>
@@ -6723,7 +6664,7 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A123" s="7" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="B123" s="1">
         <v>633</v>
@@ -6738,7 +6679,7 @@
         <v>149</v>
       </c>
       <c r="F123" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="G123" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
- added buffering to TelmetryValue - added changed flag to TelemetryValue - added interface for calculations - modified ProtocolHeader
</commit_message>
<xml_diff>
--- a/docs/TelemetryValues.xlsx
+++ b/docs/TelemetryValues.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Code\Telemetry Reader\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741BF660-DF4C-40F4-9C6B-32F0247E05D0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EFCBD3-287A-4173-9795-1FE5D7310000}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17565" xr2:uid="{A755A8CE-3DDE-4B04-B560-9846973B1798}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17565" activeTab="1" xr2:uid="{A755A8CE-3DDE-4B04-B560-9846973B1798}"/>
   </bookViews>
   <sheets>
-    <sheet name="Car" sheetId="1" r:id="rId1"/>
-    <sheet name="Driver" sheetId="2" r:id="rId2"/>
-    <sheet name="Session" sheetId="3" r:id="rId3"/>
+    <sheet name="Connection" sheetId="4" r:id="rId1"/>
+    <sheet name="Car" sheetId="1" r:id="rId2"/>
+    <sheet name="Driver" sheetId="2" r:id="rId3"/>
+    <sheet name="Session" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="178">
   <si>
     <t>Title</t>
   </si>
@@ -574,7 +574,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,6 +598,13 @@
     </font>
     <font>
       <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri Light"/>
@@ -631,7 +638,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -655,12 +662,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="45"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -3626,11 +3658,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7F112C2C-E4E7-47E6-BD1D-5458D46AA043}" name="Car" displayName="Car" ref="A1:I1048576" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7EBC1570-10BE-43E3-9EAD-E8CBDCA6872A}" name="Tabelle2" displayName="Tabelle2" ref="A1:I1048576" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:I1048576" xr:uid="{73967548-ED62-4A98-B0A4-61752DBF3F85}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{D40D18F1-A38C-46ED-9983-2D61B6E5BCDF}" name="Title"/>
+    <tableColumn id="2" xr3:uid="{1D2DD01F-616D-4BFE-AC83-F958B92F7610}" name="UID"/>
+    <tableColumn id="3" xr3:uid="{7520960B-4F1F-4A88-9EF5-B7152AC56937}" name="Datapool type"/>
+    <tableColumn id="4" xr3:uid="{980E0F7B-8CD3-47F0-8B40-A7B35B51A650}" name="Protocol type"/>
+    <tableColumn id="5" xr3:uid="{C1F71C5B-D922-4607-B2E3-9EC93B97CBAD}" name="Class"/>
+    <tableColumn id="6" xr3:uid="{71D06500-37A1-4355-8EC2-F945224E2F68}" name="Subclass (optional)"/>
+    <tableColumn id="7" xr3:uid="{C26A0372-0875-4564-BFBD-94232288FAAF}" name="Unit"/>
+    <tableColumn id="8" xr3:uid="{FCD3522E-A053-4321-A850-445DB710E4AE}" name="Description"/>
+    <tableColumn id="9" xr3:uid="{4DF988C7-087B-46F5-BA0B-282ED19C293D}" name="Calculated"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7F112C2C-E4E7-47E6-BD1D-5458D46AA043}" name="Car" displayName="Car" ref="A1:I1048576" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:I1048576" xr:uid="{9678F357-7121-4304-BFD9-FB28117FA38B}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{225A2593-5CB2-4579-B038-D91A1EEA85E3}" name="Title" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{615A14A2-858D-4418-8E7A-591D5EB29874}" name="UID" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{225A2593-5CB2-4579-B038-D91A1EEA85E3}" name="Title" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{615A14A2-858D-4418-8E7A-591D5EB29874}" name="UID" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{7DAC4DC9-1323-4BBD-ADF0-ABBE384B817C}" name="Datapool type"/>
     <tableColumn id="4" xr3:uid="{7C47352C-9903-4C70-AD6A-6DE0583434F0}" name="Protocol type"/>
     <tableColumn id="5" xr3:uid="{3188CD3B-5071-4277-9664-BF3A24A15BB0}" name="Class"/>
@@ -3881,14 +3931,1078 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36EC40CC-B9E4-4610-8236-A0356EF209BF}">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:I202"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.625" customWidth="1"/>
+    <col min="3" max="3" width="18.875" customWidth="1"/>
+    <col min="4" max="4" width="20.875" customWidth="1"/>
+    <col min="6" max="6" width="28" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="16.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="12" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B100">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B101">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B102">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B103">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B104">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B105">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B106">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B107">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B108">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B109">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B110">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B111">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B112">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B113">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B114">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B116">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B117">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B118">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B119">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B120">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B121">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B122">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B123">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B124">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B125">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B134">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B135">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B136">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B137">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B138">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B139">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B140">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B141">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B142">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B143">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B144">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B145">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B146">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B147">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B148">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B149">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B150">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B151">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B152">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B153">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B154">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B155">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B156">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B157">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B158">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B159">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B160">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B161">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B162">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B163">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B164">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B165">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B166">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B167">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B168">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B169">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B170">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B171">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B172">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B173">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B174">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B175">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B176">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B177">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B178">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B179">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B180">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B181">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B182">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B183">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B184">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B185">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B186">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B187">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B188">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B189">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B190">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B191">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B192">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B193">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B194">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B195">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B196">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B197">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B198">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B199">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B200">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B201">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B202">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF4688A-5DB6-487C-AE3E-517A2EF5E02E}">
   <sheetPr>
-    <tabColor rgb="FFFFC000"/>
+    <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:I1538"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -13770,8 +14884,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0297E23E-C423-47C8-B358-BA9F89D11940}">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13782,11 +14899,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD27DAF-1F79-4D5F-AF74-2B442D466FA5}">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
- added fuel properties to Car - modified changed property on TelmetryValue, it is now calculated based on the last two values - added calculations, packet conversion and sending to ProtocolProcessor - the processor will only convert and send, if any connection is present - packet converter is now able to skip values that did not change to reduce outgoing data
</commit_message>
<xml_diff>
--- a/docs/TelemetryValues.xlsx
+++ b/docs/TelemetryValues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Code\Telemetry Reader\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EFCBD3-287A-4173-9795-1FE5D7310000}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AE9D39-DBA3-4628-9064-7324D969B86F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17565" activeTab="1" xr2:uid="{A755A8CE-3DDE-4B04-B560-9846973B1798}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17565" xr2:uid="{A755A8CE-3DDE-4B04-B560-9846973B1798}"/>
   </bookViews>
   <sheets>
     <sheet name="Connection" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="180">
   <si>
     <t>Title</t>
   </si>
@@ -568,13 +568,19 @@
   </si>
   <si>
     <t>Wing Rear</t>
+  </si>
+  <si>
+    <t>Game ID</t>
+  </si>
+  <si>
+    <t>Reserved</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -611,6 +617,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -638,7 +652,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -662,36 +676,149 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="45"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="45"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="13">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
+        <b/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="16"/>
+        <sz val="14"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -732,6 +859,25 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2049,8 +2195,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="0" y="57162"/>
-          <a:ext cx="6596063" cy="3695674"/>
+          <a:off x="0" y="68648"/>
+          <a:ext cx="6613993" cy="3695674"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -2091,7 +2237,7 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="511928" tIns="708152" rIns="511928" bIns="113792" numCol="1" spcCol="1270" anchor="t" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="513319" tIns="708152" rIns="513319" bIns="113792" numCol="1" spcCol="1270" anchor="t" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -2241,8 +2387,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="180408" y="237570"/>
-        <a:ext cx="6235247" cy="3334858"/>
+        <a:off x="180408" y="249056"/>
+        <a:ext cx="6253177" cy="3334858"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{4A60E55B-EC82-44B0-A838-A5F0B91A2AD9}">
@@ -2252,8 +2398,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="714274" y="0"/>
-          <a:ext cx="4617244" cy="765347"/>
+          <a:off x="716216" y="0"/>
+          <a:ext cx="4629795" cy="765347"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -2325,7 +2471,7 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="174521" tIns="0" rIns="174521" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="174995" tIns="0" rIns="174995" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -2349,8 +2495,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="751635" y="37361"/>
-        <a:ext cx="4542522" cy="690625"/>
+        <a:off x="753577" y="37361"/>
+        <a:ext cx="4555073" cy="690625"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -3658,29 +3804,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7EBC1570-10BE-43E3-9EAD-E8CBDCA6872A}" name="Tabelle2" displayName="Tabelle2" ref="A1:I1048576" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7EBC1570-10BE-43E3-9EAD-E8CBDCA6872A}" name="Tabelle2" displayName="Tabelle2" ref="A1:I1048576" totalsRowShown="0" headerRowDxfId="12">
   <autoFilter ref="A1:I1048576" xr:uid="{73967548-ED62-4A98-B0A4-61752DBF3F85}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D40D18F1-A38C-46ED-9983-2D61B6E5BCDF}" name="Title"/>
-    <tableColumn id="2" xr3:uid="{1D2DD01F-616D-4BFE-AC83-F958B92F7610}" name="UID"/>
-    <tableColumn id="3" xr3:uid="{7520960B-4F1F-4A88-9EF5-B7152AC56937}" name="Datapool type"/>
-    <tableColumn id="4" xr3:uid="{980E0F7B-8CD3-47F0-8B40-A7B35B51A650}" name="Protocol type"/>
-    <tableColumn id="5" xr3:uid="{C1F71C5B-D922-4607-B2E3-9EC93B97CBAD}" name="Class"/>
-    <tableColumn id="6" xr3:uid="{71D06500-37A1-4355-8EC2-F945224E2F68}" name="Subclass (optional)"/>
-    <tableColumn id="7" xr3:uid="{C26A0372-0875-4564-BFBD-94232288FAAF}" name="Unit"/>
-    <tableColumn id="8" xr3:uid="{FCD3522E-A053-4321-A850-445DB710E4AE}" name="Description"/>
-    <tableColumn id="9" xr3:uid="{4DF988C7-087B-46F5-BA0B-282ED19C293D}" name="Calculated"/>
+    <tableColumn id="1" xr3:uid="{D40D18F1-A38C-46ED-9983-2D61B6E5BCDF}" name="Title" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{1D2DD01F-616D-4BFE-AC83-F958B92F7610}" name="UID" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{7520960B-4F1F-4A88-9EF5-B7152AC56937}" name="Datapool type" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{980E0F7B-8CD3-47F0-8B40-A7B35B51A650}" name="Protocol type" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{C1F71C5B-D922-4607-B2E3-9EC93B97CBAD}" name="Class" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{71D06500-37A1-4355-8EC2-F945224E2F68}" name="Subclass (optional)" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{C26A0372-0875-4564-BFBD-94232288FAAF}" name="Unit" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{FCD3522E-A053-4321-A850-445DB710E4AE}" name="Description" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{4DF988C7-087B-46F5-BA0B-282ED19C293D}" name="Calculated" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7F112C2C-E4E7-47E6-BD1D-5458D46AA043}" name="Car" displayName="Car" ref="A1:I1048576" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7F112C2C-E4E7-47E6-BD1D-5458D46AA043}" name="Car" displayName="Car" ref="A1:I1048576" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A1:I1048576" xr:uid="{9678F357-7121-4304-BFD9-FB28117FA38B}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{225A2593-5CB2-4579-B038-D91A1EEA85E3}" name="Title" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{615A14A2-858D-4418-8E7A-591D5EB29874}" name="UID" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{225A2593-5CB2-4579-B038-D91A1EEA85E3}" name="Title" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{615A14A2-858D-4418-8E7A-591D5EB29874}" name="UID" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{7DAC4DC9-1323-4BBD-ADF0-ABBE384B817C}" name="Datapool type"/>
     <tableColumn id="4" xr3:uid="{7C47352C-9903-4C70-AD6A-6DE0583434F0}" name="Protocol type"/>
     <tableColumn id="5" xr3:uid="{3188CD3B-5071-4277-9664-BF3A24A15BB0}" name="Class"/>
@@ -3937,1051 +4083,1093 @@
   </sheetPr>
   <dimension ref="A1:I202"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.625" customWidth="1"/>
-    <col min="3" max="3" width="18.875" customWidth="1"/>
-    <col min="4" max="4" width="20.875" customWidth="1"/>
-    <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="16.875" customWidth="1"/>
+    <col min="1" max="1" width="27.625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="11" style="12"/>
+    <col min="3" max="3" width="18.875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="20.875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="11" style="12"/>
+    <col min="6" max="6" width="28" style="12" customWidth="1"/>
+    <col min="7" max="7" width="11" style="12"/>
+    <col min="8" max="8" width="18" style="12" customWidth="1"/>
+    <col min="9" max="9" width="16.875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="12" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:9" s="11" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="B4" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" s="12">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" s="12">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="B7" s="12">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="B8" s="12">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" s="12">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="B10" s="12">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" s="12">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12" s="12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13">
+      <c r="C12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="12">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="12">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="12">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="12">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="12">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="12">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="12">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="12">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="12">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="12">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="12">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="12">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="12">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="12">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" s="12">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" s="12">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" s="12">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" s="12">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B32" s="12">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="12">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="12">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" s="12">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="12">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" s="12">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" s="12">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="12">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" s="12">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" s="12">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" s="12">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" s="12">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44" s="12">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45" s="12">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" s="12">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" s="12">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B48" s="12">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="12">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" s="12">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" s="12">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" s="12">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" s="12">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54" s="12">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B55" s="12">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B56" s="12">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B57" s="12">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B58" s="12">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B59" s="12">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B60" s="12">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B61" s="12">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B62" s="12">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B63">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B63" s="12">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B64">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B64" s="12">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65" s="12">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B66" s="12">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B67" s="12">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B68" s="12">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69" s="12">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B70" s="12">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B71" s="12">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B72" s="12">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B73" s="12">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B74" s="12">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B75" s="12">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B76" s="12">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B77" s="12">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B78" s="12">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B79" s="12">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B80" s="12">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B81" s="12">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B82" s="12">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B83" s="12">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B84" s="12">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B85" s="12">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B86" s="12">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B87" s="12">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B88" s="12">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B89" s="12">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B90" s="12">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B91" s="12">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B92" s="12">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B93" s="12">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B94" s="12">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B95" s="12">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B96" s="12">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B97" s="12">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B98" s="12">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B99" s="12">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B100" s="12">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B101" s="12">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B102" s="12">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B103" s="12">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B104">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B104" s="12">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B105" s="12">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B106" s="12">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B107" s="12">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B108" s="12">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B109" s="12">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B110">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B110" s="12">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B111" s="12">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B112">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B112" s="12">
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B113" s="12">
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B114" s="12">
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B115" s="12">
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B116" s="12">
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B117" s="12">
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B118" s="12">
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B119" s="12">
         <v>117</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B120" s="12">
         <v>118</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B121" s="12">
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B122">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B122" s="12">
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B123">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B123" s="12">
         <v>121</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B124">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B124" s="12">
         <v>122</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B125">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B125" s="12">
         <v>123</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B126">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B126" s="12">
         <v>124</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B127">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B127" s="12">
         <v>125</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B128">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B128" s="12">
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B129">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B129" s="12">
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B130">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B130" s="12">
         <v>128</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B131">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B131" s="12">
         <v>129</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B132">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B132" s="12">
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B133">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B133" s="12">
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B134">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B134" s="12">
         <v>132</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B135">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B135" s="12">
         <v>133</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B136">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B136" s="12">
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B137">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B137" s="12">
         <v>135</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B138">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B138" s="12">
         <v>136</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B139">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B139" s="12">
         <v>137</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B140">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B140" s="12">
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B141">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B141" s="12">
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B142">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B142" s="12">
         <v>140</v>
       </c>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B143">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B143" s="12">
         <v>141</v>
       </c>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B144">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B144" s="12">
         <v>142</v>
       </c>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B145">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B145" s="12">
         <v>143</v>
       </c>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B146">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B146" s="12">
         <v>144</v>
       </c>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B147">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B147" s="12">
         <v>145</v>
       </c>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B148">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B148" s="12">
         <v>146</v>
       </c>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B149">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B149" s="12">
         <v>147</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B150">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B150" s="12">
         <v>148</v>
       </c>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B151">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B151" s="12">
         <v>149</v>
       </c>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B152">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B152" s="12">
         <v>150</v>
       </c>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B153">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B153" s="12">
         <v>151</v>
       </c>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B154">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B154" s="12">
         <v>152</v>
       </c>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B155">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B155" s="12">
         <v>153</v>
       </c>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B156">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B156" s="12">
         <v>154</v>
       </c>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B157">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B157" s="12">
         <v>155</v>
       </c>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B158">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B158" s="12">
         <v>156</v>
       </c>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B159">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B159" s="12">
         <v>157</v>
       </c>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B160">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B160" s="12">
         <v>158</v>
       </c>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B161">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B161" s="12">
         <v>159</v>
       </c>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B162">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B162" s="12">
         <v>160</v>
       </c>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B163">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B163" s="12">
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B164">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B164" s="12">
         <v>162</v>
       </c>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B165">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B165" s="12">
         <v>163</v>
       </c>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B166">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B166" s="12">
         <v>164</v>
       </c>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B167">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B167" s="12">
         <v>165</v>
       </c>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B168">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B168" s="12">
         <v>166</v>
       </c>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B169">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B169" s="12">
         <v>167</v>
       </c>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B170">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B170" s="12">
         <v>168</v>
       </c>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B171">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B171" s="12">
         <v>169</v>
       </c>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B172">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B172" s="12">
         <v>170</v>
       </c>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B173">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B173" s="12">
         <v>171</v>
       </c>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B174">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B174" s="12">
         <v>172</v>
       </c>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B175">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B175" s="12">
         <v>173</v>
       </c>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B176">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B176" s="12">
         <v>174</v>
       </c>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B177">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B177" s="12">
         <v>175</v>
       </c>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B178">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B178" s="12">
         <v>176</v>
       </c>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B179">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B179" s="12">
         <v>177</v>
       </c>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B180">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B180" s="12">
         <v>178</v>
       </c>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B181">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B181" s="12">
         <v>179</v>
       </c>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B182">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B182" s="12">
         <v>180</v>
       </c>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B183">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B183" s="12">
         <v>181</v>
       </c>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B184">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B184" s="12">
         <v>182</v>
       </c>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B185">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B185" s="12">
         <v>183</v>
       </c>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B186">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B186" s="12">
         <v>184</v>
       </c>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B187">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B187" s="12">
         <v>185</v>
       </c>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B188">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B188" s="12">
         <v>186</v>
       </c>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B189">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B189" s="12">
         <v>187</v>
       </c>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B190">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B190" s="12">
         <v>188</v>
       </c>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B191">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B191" s="12">
         <v>189</v>
       </c>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B192">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B192" s="12">
         <v>190</v>
       </c>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B193">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B193" s="12">
         <v>191</v>
       </c>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B194">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B194" s="12">
         <v>192</v>
       </c>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B195">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B195" s="12">
         <v>193</v>
       </c>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B196">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B196" s="12">
         <v>194</v>
       </c>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B197">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B197" s="12">
         <v>195</v>
       </c>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B198">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B198" s="12">
         <v>196</v>
       </c>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B199">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B199" s="12">
         <v>197</v>
       </c>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B200">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B200" s="12">
         <v>198</v>
       </c>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B201">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B201" s="12">
         <v>199</v>
       </c>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B202">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B202" s="12">
         <v>200</v>
       </c>
     </row>
@@ -5001,8 +5189,8 @@
   </sheetPr>
   <dimension ref="A1:I1538"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.35"/>

</xml_diff>